<commit_message>
fix clsMongoDb -- thêm mới tính năng tổng hợp dữ liệu cho các báo cáo theo quý
</commit_message>
<xml_diff>
--- a/ReportWebApplication/Temp/201706/G02005-01912001-01912001-201706-BT-M-01.xlsx
+++ b/ReportWebApplication/Temp/201706/G02005-01912001-01912001-201706-BT-M-01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>G02005</t>
   </si>
@@ -113,6 +113,12 @@
     <t xml:space="preserve">   1. Chi nộp thuế và các khoản phí, lệ phí</t>
   </si>
   <si>
+    <t>00,0</t>
+  </si>
+  <si>
+    <t>06,1</t>
+  </si>
+  <si>
     <t>R-103</t>
   </si>
   <si>
@@ -155,9 +161,6 @@
     <t xml:space="preserve">                       - Chi trợ cấp</t>
   </si>
   <si>
-    <t>00,0</t>
-  </si>
-  <si>
     <t>R-107</t>
   </si>
   <si>
@@ -230,7 +233,7 @@
     <t>01,9</t>
   </si>
   <si>
-    <t>02,4</t>
+    <t>00,5</t>
   </si>
   <si>
     <t>R-114</t>
@@ -251,28 +254,28 @@
     <t xml:space="preserve">   6. Chi phí dự phòng (không tính chi phí dự phòng rủi ro tín dụng; chi phí dự phòng rủi ro chứng khoán)</t>
   </si>
   <si>
-    <t>15,8</t>
-  </si>
-  <si>
-    <t>157,3</t>
-  </si>
-  <si>
     <t>R-116</t>
   </si>
   <si>
     <t xml:space="preserve">   7. Chi phí hoạt động khác</t>
   </si>
   <si>
+    <t>05,9</t>
+  </si>
+  <si>
+    <t>03,0</t>
+  </si>
+  <si>
     <t>R-117</t>
   </si>
   <si>
     <t>Tổng</t>
   </si>
   <si>
-    <t>4975,2</t>
-  </si>
-  <si>
-    <t>5153,3</t>
+    <t>4965,4</t>
+  </si>
+  <si>
+    <t>4999,0</t>
   </si>
   <si>
     <t>R-118</t>
@@ -299,6 +302,12 @@
     <t xml:space="preserve">      1. Tổng quỹ lương</t>
   </si>
   <si>
+    <t>3241,7</t>
+  </si>
+  <si>
+    <t>3024,4</t>
+  </si>
+  <si>
     <t>R-122</t>
   </si>
   <si>
@@ -323,10 +332,10 @@
     <t xml:space="preserve">      5. Tiền lương bình quân</t>
   </si>
   <si>
-    <t>34,2</t>
-  </si>
-  <si>
-    <t>34,4</t>
+    <t>30,0</t>
+  </si>
+  <si>
+    <t>28,0</t>
   </si>
   <si>
     <t>R-126</t>
@@ -1035,231 +1044,235 @@
       <c r="B19" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="C19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" ht="28.5">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" ht="28.5">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" ht="28.5">
       <c r="A31" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" ht="42.75">
       <c r="A32" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="C33" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="D33" s="9" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" ht="28.5">
       <c r="A35" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C36" s="8">
         <v>108</v>
@@ -1270,104 +1283,104 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="D43" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" ht="300" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>

</xml_diff>